<commit_message>
Areas can have multi-sheet references too, so add FormulaParser support to these as well
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1613437 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/55906-MultiSheetRefs.xlsx
+++ b/test-data/spreadsheet/55906-MultiSheetRefs.xlsx
@@ -372,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>11</v>
       </c>
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>SUM(Sheet1:Sheet3!A1)</f>
         <v>66</v>
@@ -412,22 +412,42 @@
         <f>COUNTA(Sheet1:Sheet3!E1)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>SUM(Sheet1:Sheet3!A1:B2)</f>
+        <v>66</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(Sheet1:Sheet3!A1:B2)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>MIN(Sheet1:Sheet3!A$1)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f>MIN(Sheet1:Sheet3!A$1:B$2)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>MAX(Sheet1:Sheet3!A$1)</f>
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f>MAX(Sheet1:Sheet3!A$1:B$2)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>COUNT(Sheet1:Sheet3!A$1)</f>
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f>COUNT(Sheet1:Sheet3!$A$1:$B$2)</f>
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More tests for #55906, and provide a new eval that lets you get at evals for many sheets
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1613438 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/55906-MultiSheetRefs.xlsx
+++ b/test-data/spreadsheet/55906-MultiSheetRefs.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,11 +414,11 @@
       </c>
       <c r="H3">
         <f>SUM(Sheet1:Sheet3!A1:B2)</f>
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="I3">
         <f>AVERAGE(Sheet1:Sheet3!A1:B2)</f>
-        <v>22</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -438,7 +438,7 @@
       </c>
       <c r="I5">
         <f>MAX(Sheet1:Sheet3!A$1:B$2)</f>
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
       </c>
       <c r="I6">
         <f>COUNT(Sheet1:Sheet3!$A$1:$B$2)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +469,9 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>22</v>
+      </c>
+      <c r="B1">
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>

</xml_diff>